<commit_message>
finished first advanced exercise
</commit_message>
<xml_diff>
--- a/spreadsheets/shopping.xlsx
+++ b/spreadsheets/shopping.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="createAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="loginDetails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>John</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>john.smith@hotmail.com</t>
-  </si>
-  <si>
     <t>johnsmith</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>dragon</t>
+  </si>
+  <si>
+    <t>#55592111880</t>
+  </si>
+  <si>
+    <t>johnsmith10@live.com</t>
   </si>
 </sst>
 </file>
@@ -171,11 +174,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -482,7 +484,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,75 +515,75 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -589,26 +591,26 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3">
         <v>1995</v>
       </c>
       <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -617,36 +619,33 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="O2" s="3"/>
       <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
         <v>17</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>18</v>
       </c>
       <c r="R2" s="3">
         <v>12345</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="3">
-        <v>55592111880</v>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="V2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -655,7 +654,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,18 +665,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>